<commit_message>
Bug Fixes: - Memb 9: Added dummy data for easier visualization.
</commit_message>
<xml_diff>
--- a/Documentation/Test Cases/Test Cases Updated 28 June 2018.xlsx
+++ b/Documentation/Test Cases/Test Cases Updated 28 June 2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\Tempest\Documentation\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAA27E2-91DD-430B-8F7B-EC8946DB6A9F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8787671-287A-499A-9F67-41655DF0133D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6600" tabRatio="845" xr2:uid="{C6E4BB7B-75ED-42D2-8931-FE7C9C9824C8}"/>
   </bookViews>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="229">
   <si>
     <t>S/N</t>
   </si>
@@ -1397,6 +1397,22 @@
   </si>
   <si>
     <t>Jacky</t>
+  </si>
+  <si>
+    <t>Check database to verify if photo is uploaded. Check with Josh where we need to show display photo.</t>
+  </si>
+  <si>
+    <t>Disabled checking for existing mobile numbers in database. Currently the form will auto populate the current email address and mobile number of the customer. If no changes, SQL query is run but no change in database is made. See updateProfile and updateProfileNoPhoto methods in CustomerDAO.</t>
+  </si>
+  <si>
+    <t>Login page - Changed "Change Password" to "Forget Password?".
+Added "Change Password" option in dropdown menu for customer.</t>
+  </si>
+  <si>
+    <t>No such function implemented</t>
+  </si>
+  <si>
+    <t>Added dummy data for easier visualisation.</t>
   </si>
 </sst>
 </file>
@@ -1599,9 +1615,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1625,6 +1638,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2040,22 +2056,22 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="O73" sqref="O73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="12" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" style="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45.7109375" style="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" style="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="44.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.28515625" style="32" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.7109375" style="16" bestFit="1" customWidth="1"/>
@@ -4715,7 +4731,7 @@
         <v>168</v>
       </c>
       <c r="L66" s="5" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="M66" s="5" t="s">
         <v>216</v>
@@ -4723,9 +4739,11 @@
       <c r="N66" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="O66" s="5"/>
-    </row>
-    <row r="67" spans="1:15" ht="24" x14ac:dyDescent="0.2">
+      <c r="O66" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
         <v>72</v>
       </c>
@@ -4759,7 +4777,7 @@
         <v>169</v>
       </c>
       <c r="L67" s="5" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="M67" s="5" t="s">
         <v>216</v>
@@ -4767,9 +4785,11 @@
       <c r="N67" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="O67" s="5"/>
-    </row>
-    <row r="68" spans="1:15" ht="24" x14ac:dyDescent="0.2">
+      <c r="O67" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
         <v>72</v>
       </c>
@@ -4803,7 +4823,7 @@
         <v>168</v>
       </c>
       <c r="L68" s="5" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="M68" s="5" t="s">
         <v>216</v>
@@ -4811,9 +4831,11 @@
       <c r="N68" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="O68" s="5"/>
-    </row>
-    <row r="69" spans="1:15" ht="24" x14ac:dyDescent="0.2">
+      <c r="O68" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
         <v>72</v>
       </c>
@@ -4847,7 +4869,7 @@
         <v>168</v>
       </c>
       <c r="L69" s="5" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="M69" s="5" t="s">
         <v>216</v>
@@ -4855,9 +4877,11 @@
       <c r="N69" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="O69" s="5"/>
-    </row>
-    <row r="70" spans="1:15" ht="24" x14ac:dyDescent="0.2">
+      <c r="O69" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
         <v>72</v>
       </c>
@@ -4891,7 +4915,7 @@
         <v>168</v>
       </c>
       <c r="L70" s="5" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="M70" s="5" t="s">
         <v>216</v>
@@ -4899,7 +4923,9 @@
       <c r="N70" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="O70" s="5"/>
+      <c r="O70" s="5" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="71" spans="1:15" ht="24" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
@@ -4918,16 +4944,16 @@
       <c r="E71" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F71" s="25" t="s">
+      <c r="F71" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="G71" s="25"/>
-      <c r="H71" s="25"/>
-      <c r="I71" s="25"/>
-      <c r="J71" s="25"/>
-      <c r="K71" s="25"/>
+      <c r="G71" s="33"/>
+      <c r="H71" s="33"/>
+      <c r="I71" s="33"/>
+      <c r="J71" s="33"/>
+      <c r="K71" s="33"/>
       <c r="L71" s="5" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="M71" s="5" t="s">
         <v>216</v>
@@ -4935,9 +4961,11 @@
       <c r="N71" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="O71" s="5"/>
-    </row>
-    <row r="72" spans="1:15" ht="24" x14ac:dyDescent="0.2">
+      <c r="O71" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
         <v>72</v>
       </c>
@@ -4971,7 +4999,7 @@
         <v>176</v>
       </c>
       <c r="L72" s="5" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="M72" s="5" t="s">
         <v>216</v>
@@ -4979,9 +5007,11 @@
       <c r="N72" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="O72" s="5"/>
-    </row>
-    <row r="73" spans="1:15" ht="24" x14ac:dyDescent="0.2">
+      <c r="O72" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
         <v>72</v>
       </c>
@@ -5015,7 +5045,7 @@
         <v>176</v>
       </c>
       <c r="L73" s="5" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="M73" s="5" t="s">
         <v>216</v>
@@ -5023,7 +5053,9 @@
       <c r="N73" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="O73" s="5"/>
+      <c r="O73" s="5" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="74" spans="1:15" ht="24" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
@@ -5059,7 +5091,7 @@
         <v>168</v>
       </c>
       <c r="L74" s="5" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="M74" s="5" t="s">
         <v>216</v>
@@ -5067,7 +5099,9 @@
       <c r="N74" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="O74" s="5"/>
+      <c r="O74" s="5" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="75" spans="1:15" ht="24" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
@@ -5103,7 +5137,7 @@
         <v>169</v>
       </c>
       <c r="L75" s="5" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="M75" s="5" t="s">
         <v>216</v>
@@ -5111,7 +5145,9 @@
       <c r="N75" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="O75" s="5"/>
+      <c r="O75" s="5" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="76" spans="1:15" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
@@ -5185,7 +5221,7 @@
         <v>169</v>
       </c>
       <c r="L77" s="5" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="M77" s="5" t="s">
         <v>216</v>
@@ -5193,7 +5229,9 @@
       <c r="N77" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="O77" s="5"/>
+      <c r="O77" s="5" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="78" spans="1:15" ht="36" x14ac:dyDescent="0.2">
       <c r="A78" s="11" t="s">
@@ -5223,7 +5261,7 @@
         <v>122</v>
       </c>
       <c r="J78" s="11"/>
-      <c r="K78" s="26" t="s">
+      <c r="K78" s="25" t="s">
         <v>201</v>
       </c>
       <c r="L78" s="5" t="s">
@@ -5265,7 +5303,7 @@
         <v>21</v>
       </c>
       <c r="J79" s="11"/>
-      <c r="K79" s="26" t="s">
+      <c r="K79" s="25" t="s">
         <v>202</v>
       </c>
       <c r="L79" s="5" t="s">
@@ -5367,10 +5405,10 @@
       <c r="A82" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B82" s="27">
+      <c r="B82" s="26">
         <v>5</v>
       </c>
-      <c r="C82" s="28" t="str">
+      <c r="C82" s="27" t="str">
         <f t="shared" si="16"/>
         <v>UT 5</v>
       </c>
@@ -5407,7 +5445,7 @@
       <c r="A83" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B83" s="29">
+      <c r="B83" s="28">
         <v>6</v>
       </c>
       <c r="C83" s="15" t="str">
@@ -5449,7 +5487,7 @@
       <c r="A84" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B84" s="29">
+      <c r="B84" s="28">
         <v>7</v>
       </c>
       <c r="C84" s="15" t="str">

</xml_diff>

<commit_message>
Updated the test cases to change status of bug 53 and 55 to fixed
</commit_message>
<xml_diff>
--- a/Documentation/Test Cases/Test Cases Updated 28 June 2018.xlsx
+++ b/Documentation/Test Cases/Test Cases Updated 28 June 2018.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\Tempest\Documentation\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacky\Documents\fyp\Tempest\Documentation\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8787671-287A-499A-9F67-41655DF0133D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CF31B8-1004-425B-9C55-0699493A9A4D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6600" tabRatio="845" xr2:uid="{C6E4BB7B-75ED-42D2-8931-FE7C9C9824C8}"/>
   </bookViews>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="230">
   <si>
     <t>S/N</t>
   </si>
@@ -1413,6 +1413,9 @@
   </si>
   <si>
     <t>Added dummy data for easier visualisation.</t>
+  </si>
+  <si>
+    <t>unable to reproduce bug to fixed it</t>
   </si>
 </sst>
 </file>
@@ -2053,33 +2056,33 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="O73" sqref="O73"/>
+      <selection pane="bottomLeft" activeCell="O83" sqref="O83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="12" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="27.3984375" defaultRowHeight="11.5" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.09765625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.59765625" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.8984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.8984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.69921875" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.3984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.8984375" style="31" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.59765625" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.296875" style="32" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.3984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.59765625" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.69921875" style="16" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="70" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="27.42578125" style="16"/>
+    <col min="16" max="16384" width="27.3984375" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="3" customFormat="1" ht="23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>70</v>
       </c>
@@ -2126,7 +2129,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="10" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" s="10" customFormat="1" ht="34.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>85</v>
       </c>
@@ -2172,7 +2175,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="10" customFormat="1" ht="48" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" s="10" customFormat="1" ht="46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>71</v>
       </c>
@@ -2218,7 +2221,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="10" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" s="10" customFormat="1" ht="34.5" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>85</v>
       </c>
@@ -2256,7 +2259,7 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" spans="1:15" s="10" customFormat="1" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" s="10" customFormat="1" ht="46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>71</v>
       </c>
@@ -2290,7 +2293,7 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:15" s="10" customFormat="1" ht="36" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" s="10" customFormat="1" ht="34.5" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>85</v>
       </c>
@@ -2336,7 +2339,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="10" customFormat="1" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" s="10" customFormat="1" ht="46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>71</v>
       </c>
@@ -2370,7 +2373,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:15" s="10" customFormat="1" ht="24" hidden="1" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" s="10" customFormat="1" ht="23" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>85</v>
       </c>
@@ -2408,7 +2411,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:15" s="10" customFormat="1" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" s="10" customFormat="1" ht="46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>71</v>
       </c>
@@ -2442,7 +2445,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:15" s="10" customFormat="1" ht="60" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" s="10" customFormat="1" ht="57.5" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>85</v>
       </c>
@@ -2488,7 +2491,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="10" customFormat="1" ht="48" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" s="10" customFormat="1" ht="46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>71</v>
       </c>
@@ -2532,7 +2535,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="10" customFormat="1" ht="48" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" s="10" customFormat="1" ht="46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>71</v>
       </c>
@@ -2576,7 +2579,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" s="10" customFormat="1" ht="57.5" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>85</v>
       </c>
@@ -2622,7 +2625,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="10" customFormat="1" ht="60" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" s="10" customFormat="1" ht="57.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>71</v>
       </c>
@@ -2669,7 +2672,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="10" customFormat="1" ht="60" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" s="10" customFormat="1" ht="57.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>71</v>
       </c>
@@ -2714,7 +2717,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="72" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="69" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>85</v>
       </c>
@@ -2752,7 +2755,7 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="1:15" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>71</v>
       </c>
@@ -2789,7 +2792,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="1:15" ht="48" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="46" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>85</v>
       </c>
@@ -2835,7 +2838,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="96" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="92" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>71</v>
       </c>
@@ -2882,7 +2885,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="48" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>71</v>
       </c>
@@ -2929,7 +2932,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="48" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>71</v>
       </c>
@@ -2976,7 +2979,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>85</v>
       </c>
@@ -3014,7 +3017,7 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
     </row>
-    <row r="23" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>85</v>
       </c>
@@ -3060,7 +3063,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>85</v>
       </c>
@@ -3106,7 +3109,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>85</v>
       </c>
@@ -3152,7 +3155,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>85</v>
       </c>
@@ -3198,7 +3201,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>85</v>
       </c>
@@ -3244,7 +3247,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="34.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>119</v>
       </c>
@@ -3282,7 +3285,7 @@
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
     </row>
-    <row r="29" spans="1:15" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="34.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>119</v>
       </c>
@@ -3320,7 +3323,7 @@
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
     </row>
-    <row r="30" spans="1:15" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="34.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>71</v>
       </c>
@@ -3355,7 +3358,7 @@
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
     </row>
-    <row r="31" spans="1:15" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="34.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>71</v>
       </c>
@@ -3390,7 +3393,7 @@
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
     </row>
-    <row r="32" spans="1:15" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="34.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>71</v>
       </c>
@@ -3425,7 +3428,7 @@
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
     </row>
-    <row r="33" spans="1:15" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="34.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>71</v>
       </c>
@@ -3460,7 +3463,7 @@
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
     </row>
-    <row r="34" spans="1:15" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="34.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>71</v>
       </c>
@@ -3495,7 +3498,7 @@
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
     </row>
-    <row r="35" spans="1:15" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="34.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>71</v>
       </c>
@@ -3530,7 +3533,7 @@
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
     </row>
-    <row r="36" spans="1:15" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="34.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>71</v>
       </c>
@@ -3565,7 +3568,7 @@
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
     </row>
-    <row r="37" spans="1:15" ht="24" hidden="1" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="23" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>71</v>
       </c>
@@ -3603,7 +3606,7 @@
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
     </row>
-    <row r="38" spans="1:15" ht="24" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" ht="23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>139</v>
       </c>
@@ -3648,7 +3651,7 @@
       </c>
       <c r="O38" s="5"/>
     </row>
-    <row r="39" spans="1:15" ht="84" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="80.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>139</v>
       </c>
@@ -3685,7 +3688,7 @@
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
     </row>
-    <row r="40" spans="1:15" ht="84" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" ht="80.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>139</v>
       </c>
@@ -3728,7 +3731,7 @@
       </c>
       <c r="O40" s="5"/>
     </row>
-    <row r="41" spans="1:15" ht="84" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" ht="80.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>139</v>
       </c>
@@ -3765,7 +3768,7 @@
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
     </row>
-    <row r="42" spans="1:15" ht="84" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" ht="80.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>139</v>
       </c>
@@ -3808,7 +3811,7 @@
       </c>
       <c r="O42" s="5"/>
     </row>
-    <row r="43" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="46" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>139</v>
       </c>
@@ -3853,7 +3856,7 @@
       </c>
       <c r="O43" s="5"/>
     </row>
-    <row r="44" spans="1:15" ht="72" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="69" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>139</v>
       </c>
@@ -3888,7 +3891,7 @@
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
     </row>
-    <row r="45" spans="1:15" ht="72" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" ht="69" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>139</v>
       </c>
@@ -3923,7 +3926,7 @@
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
     </row>
-    <row r="46" spans="1:15" ht="72" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" ht="69" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>139</v>
       </c>
@@ -3958,7 +3961,7 @@
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
     </row>
-    <row r="47" spans="1:15" ht="24" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" ht="23" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>139</v>
       </c>
@@ -4003,7 +4006,7 @@
       </c>
       <c r="O47" s="5"/>
     </row>
-    <row r="48" spans="1:15" ht="108" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="103.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>139</v>
       </c>
@@ -4038,7 +4041,7 @@
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
     </row>
-    <row r="49" spans="1:15" ht="84" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" ht="80.5" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>139</v>
       </c>
@@ -4083,7 +4086,7 @@
       </c>
       <c r="O49" s="5"/>
     </row>
-    <row r="50" spans="1:15" ht="72" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" ht="69" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>139</v>
       </c>
@@ -4118,7 +4121,7 @@
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
     </row>
-    <row r="51" spans="1:15" ht="72" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" ht="69" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>139</v>
       </c>
@@ -4153,7 +4156,7 @@
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
     </row>
-    <row r="52" spans="1:15" ht="24" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" ht="23" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>139</v>
       </c>
@@ -4198,7 +4201,7 @@
       </c>
       <c r="O52" s="5"/>
     </row>
-    <row r="53" spans="1:15" ht="60" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" ht="57.5" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>139</v>
       </c>
@@ -4233,7 +4236,7 @@
         <v>175</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="M53" s="5" t="s">
         <v>216</v>
@@ -4243,7 +4246,7 @@
       </c>
       <c r="O53" s="5"/>
     </row>
-    <row r="54" spans="1:15" ht="120" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" ht="115" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>139</v>
       </c>
@@ -4280,7 +4283,7 @@
       <c r="N54" s="5"/>
       <c r="O54" s="5"/>
     </row>
-    <row r="55" spans="1:15" ht="132" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" ht="126.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>139</v>
       </c>
@@ -4313,7 +4316,7 @@
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="M55" s="5" t="s">
         <v>216</v>
@@ -4323,7 +4326,7 @@
       </c>
       <c r="O55" s="5"/>
     </row>
-    <row r="56" spans="1:15" ht="72" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" ht="69" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>139</v>
       </c>
@@ -4368,7 +4371,7 @@
       </c>
       <c r="O56" s="5"/>
     </row>
-    <row r="57" spans="1:15" ht="108" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" ht="103.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>139</v>
       </c>
@@ -4403,7 +4406,7 @@
       <c r="N57" s="5"/>
       <c r="O57" s="5"/>
     </row>
-    <row r="58" spans="1:15" ht="24" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" ht="23" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>139</v>
       </c>
@@ -4448,7 +4451,7 @@
       </c>
       <c r="O58" s="5"/>
     </row>
-    <row r="59" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" ht="46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>139</v>
       </c>
@@ -4487,7 +4490,7 @@
       <c r="N59" s="5"/>
       <c r="O59" s="5"/>
     </row>
-    <row r="60" spans="1:15" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" ht="46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
         <v>139</v>
       </c>
@@ -4522,7 +4525,7 @@
       <c r="N60" s="5"/>
       <c r="O60" s="5"/>
     </row>
-    <row r="61" spans="1:15" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" ht="46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
         <v>139</v>
       </c>
@@ -4557,7 +4560,7 @@
       <c r="N61" s="5"/>
       <c r="O61" s="5"/>
     </row>
-    <row r="62" spans="1:15" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" ht="46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
         <v>139</v>
       </c>
@@ -4592,7 +4595,7 @@
       <c r="N62" s="5"/>
       <c r="O62" s="5"/>
     </row>
-    <row r="63" spans="1:15" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" ht="46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>139</v>
       </c>
@@ -4627,7 +4630,7 @@
       <c r="N63" s="5"/>
       <c r="O63" s="5"/>
     </row>
-    <row r="64" spans="1:15" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" ht="46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
         <v>139</v>
       </c>
@@ -4662,7 +4665,7 @@
       <c r="N64" s="5"/>
       <c r="O64" s="5"/>
     </row>
-    <row r="65" spans="1:15" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" ht="46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>139</v>
       </c>
@@ -4697,7 +4700,7 @@
       <c r="N65" s="5"/>
       <c r="O65" s="5"/>
     </row>
-    <row r="66" spans="1:15" ht="24" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" ht="23" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>72</v>
       </c>
@@ -4743,7 +4746,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" ht="46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
         <v>72</v>
       </c>
@@ -4789,7 +4792,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" ht="46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>72</v>
       </c>
@@ -4835,7 +4838,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15" ht="46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
         <v>72</v>
       </c>
@@ -4881,7 +4884,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15" ht="46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>72</v>
       </c>
@@ -4927,7 +4930,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="24" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:15" ht="23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>72</v>
       </c>
@@ -4965,7 +4968,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:15" ht="46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>72</v>
       </c>
@@ -5011,7 +5014,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15" ht="46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>72</v>
       </c>
@@ -5057,7 +5060,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="24" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15" ht="23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>72</v>
       </c>
@@ -5103,7 +5106,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="24" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:15" ht="23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>72</v>
       </c>
@@ -5149,7 +5152,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15" ht="23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
         <v>72</v>
       </c>
@@ -5187,7 +5190,7 @@
       <c r="N76" s="5"/>
       <c r="O76" s="5"/>
     </row>
-    <row r="77" spans="1:15" ht="24" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15" ht="23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>72</v>
       </c>
@@ -5233,7 +5236,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="36" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15" ht="34.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>182</v>
       </c>
@@ -5275,7 +5278,7 @@
       </c>
       <c r="O78" s="5"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
         <v>182</v>
       </c>
@@ -5317,7 +5320,7 @@
       </c>
       <c r="O79" s="5"/>
     </row>
-    <row r="80" spans="1:15" ht="108" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:15" ht="103.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
         <v>182</v>
       </c>
@@ -5359,7 +5362,7 @@
       </c>
       <c r="O80" s="5"/>
     </row>
-    <row r="81" spans="1:15" ht="36" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" ht="34.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
         <v>182</v>
       </c>
@@ -5401,7 +5404,7 @@
       </c>
       <c r="O81" s="5"/>
     </row>
-    <row r="82" spans="1:15" ht="24" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15" ht="23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>182</v>
       </c>
@@ -5441,7 +5444,7 @@
       </c>
       <c r="O82" s="5"/>
     </row>
-    <row r="83" spans="1:15" ht="60" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" ht="57.5" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>182</v>
       </c>
@@ -5481,9 +5484,11 @@
       <c r="N83" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="O83" s="5"/>
-    </row>
-    <row r="84" spans="1:15" ht="72" x14ac:dyDescent="0.2">
+      <c r="O83" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" ht="69" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
         <v>182</v>
       </c>
@@ -5525,7 +5530,7 @@
       </c>
       <c r="O84" s="5"/>
     </row>
-    <row r="85" spans="1:15" ht="36" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15" ht="34.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
         <v>182</v>
       </c>
@@ -5574,6 +5579,11 @@
         <filter val="N due to UI"/>
         <filter val="TBC"/>
         <filter val="Y for logic, N for UI"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="13">
+      <filters>
+        <filter val="Jacky"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5602,19 +5612,19 @@
       <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="59" ht="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="13" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>